<commit_message>
Refazendo teste da densenet
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Pessoal\FerPlus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF07D20A-0EE8-4B05-A840-F4503BD8EA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498FF0EC-146A-4A43-B8A9-2011D25961C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resultados" sheetId="1" r:id="rId1"/>
     <sheet name="resultados-balanceados" sheetId="37" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'resultados-balanceados'!$B$1:$B$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'resultados-balanceados'!$B$1:$B$95</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="36">
   <si>
     <t>modelo</t>
   </si>
@@ -127,11 +127,20 @@
   <si>
     <t>weighted</t>
   </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Comparador multi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,6 +153,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -195,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -204,199 +214,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <b/>
@@ -893,9 +718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1939,7 +1766,7 @@
         <v>0.13333334028720861</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2004,7 +1831,7 @@
         <v>0.13333334028720861</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2069,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2134,7 +1961,7 @@
         <v>6.6666670143604279E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2199,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2264,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2329,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2394,7 +2221,7 @@
         <v>6.6666670143604279E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2459,7 +2286,7 @@
         <v>6.6666670143604279E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2524,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2587,6 +2414,148 @@
       </c>
       <c r="U26">
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.90668202764976957</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.90998268897864976</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.82788527011871338</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.88318228721618652</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.78842675685882568</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.47179487347602839</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.63636362552642822</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.32867133617401117</v>
+      </c>
+      <c r="M29" s="2">
+        <v>7.2727270424365997E-2</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0.83080112934112549</v>
+      </c>
+      <c r="O29" s="2">
+        <v>0.89009898900985718</v>
+      </c>
+      <c r="P29" s="2">
+        <v>0.75963300466537476</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>0.44476744532585138</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0.68733853101730347</v>
+      </c>
+      <c r="S29" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="T29" s="2">
+        <v>0.29213482141494751</v>
+      </c>
+      <c r="U29" s="2">
+        <v>0.1025641039013863</v>
+      </c>
+      <c r="V29">
+        <v>64</v>
+      </c>
+      <c r="W29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.907258064516129</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.90767455279861509</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.80920612812042236</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.86002016067504883</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.79746836423873901</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0.60000002384185791</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0.61616164445877075</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0.26666668057441711</v>
+      </c>
+      <c r="L30" s="5">
+        <v>0.20979021489620209</v>
+      </c>
+      <c r="M30" s="5">
+        <v>1.8181817606091499E-2</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0.81491714715957642</v>
+      </c>
+      <c r="O30" s="5">
+        <v>0.86336636543273926</v>
+      </c>
+      <c r="P30" s="5">
+        <v>0.80000001192092896</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>0.53488373756408691</v>
+      </c>
+      <c r="R30" s="5">
+        <v>0.63824290037155151</v>
+      </c>
+      <c r="S30" s="5">
+        <v>0.17499999701976779</v>
+      </c>
+      <c r="T30" s="5">
+        <v>0.19662921130657199</v>
+      </c>
+      <c r="U30" s="5">
+        <v>2.5641025975346569E-2</v>
+      </c>
+      <c r="V30">
+        <v>64</v>
+      </c>
+      <c r="W30" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2596,11 +2565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:W1048565"/>
+  <dimension ref="A1:W1048566"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,24 +2576,24 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2711,58 +2679,58 @@
       <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>0.85271074898151045</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>0.84762511954096276</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>0.87033897638320923</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>0.92459398508071899</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="4">
         <v>0.89781022071838379</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="4">
         <v>0.69252872467041016</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="4">
         <v>0.78892731666564941</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="4">
         <v>0.40000000596046448</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="4">
         <v>0.69999998807907104</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <v>0.4375</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>0.8790397047996521</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="4">
         <v>0.91255605220794678</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="4">
         <v>0.8807106614112854</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="4">
         <v>0.6963350772857666</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="4">
         <v>0.832713782787323</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="4">
         <v>0.5</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="4">
         <v>0.52325582504272461</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="4">
         <v>0.20000000298023221</v>
       </c>
       <c r="V2">
@@ -2772,7 +2740,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2782,58 +2750,58 @@
       <c r="C3">
         <v>35</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>0.85678470698840492</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>0.84698756773987882</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>0.89576274156570435</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>0.93271464109420776</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>0.9051094651222229</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>0.64942526817321777</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <v>0.754325270652771</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <v>0.47999998927116388</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="4">
         <v>0.64999997615814209</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>0.375</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>0.90858727693557739</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="4">
         <v>0.90134531259536743</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="4">
         <v>0.87817257642745972</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="4">
         <v>0.63874346017837524</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="4">
         <v>0.82527881860733032</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="4">
         <v>0.625</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="4">
         <v>0.5116279125213623</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="4">
         <v>0.20000000298023221</v>
       </c>
       <c r="V3">
@@ -2843,7 +2811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2853,58 +2821,58 @@
       <c r="C4">
         <v>22</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>0.85803823252898781</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>0.85017532674529805</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>0.87033897638320923</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>0.93619489669799805</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>0.88077861070632935</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>0.75287353992462158</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>0.76470589637756348</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>0.51999998092651367</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>0.64999997615814209</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>0.4375</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>0.88919669389724731</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="4">
         <v>0.93049329519271851</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="4">
         <v>0.85279190540313721</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="4">
         <v>0.73036646842956543</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="4">
         <v>0.77323418855667114</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <v>0.5</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="4">
         <v>0.46511629223823547</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="4">
         <v>0.20000000298023221</v>
       </c>
       <c r="V4">
@@ -2914,7 +2882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2924,58 +2892,58 @@
       <c r="C5">
         <v>22</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>0.84362268881228453</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>0.83869939432578899</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>0.85677963495254517</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>0.92459398508071899</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>0.87834548950195313</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>0.68678158521652222</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>0.78200691938400269</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>0.51999998092651367</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>0.60000002384185791</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>0.5625</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>0.86611264944076538</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="4">
         <v>0.92376679182052612</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="4">
         <v>0.87309646606445313</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="4">
         <v>0.67539268732070923</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="4">
         <v>0.80297398567199707</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="4">
         <v>0.625</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="4">
         <v>0.43023255467414862</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="4">
         <v>0.26666668057441711</v>
       </c>
       <c r="V5">
@@ -2995,58 +2963,58 @@
       <c r="C6">
         <v>29</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>0.85741146975869631</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>0.84858144724258844</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>0.86694914102554321</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>0.9385150671005249</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>0.89537709951400757</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>0.72413790225982666</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="4">
         <v>0.79930794239044189</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <v>0.40000000596046448</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="4">
         <v>0.61666667461395264</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="4">
         <v>0.375</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="4">
         <v>0.86888271570205688</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="4">
         <v>0.93161433935165405</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="4">
         <v>0.89086294174194336</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="4">
         <v>0.69109946489334106</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="4">
         <v>0.81784385442733765</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="4">
         <v>0.5625</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="4">
         <v>0.5</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="4">
         <v>0.20000000298023221</v>
       </c>
       <c r="V6">
@@ -3056,7 +3024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3066,58 +3034,58 @@
       <c r="C7">
         <v>24</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>0.85177060482607336</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>0.85113165444692385</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>0.85423725843429565</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>0.93503481149673462</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>0.87834548950195313</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <v>0.7183908224105835</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <v>0.79584777355194092</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>0.51999998092651367</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="4">
         <v>0.69999998807907104</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <v>0.5</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="4">
         <v>0.87811636924743652</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="4">
         <v>0.92264574766159058</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="4">
         <v>0.89086294174194336</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="4">
         <v>0.69895285367965698</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="4">
         <v>0.832713782787323</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="4">
         <v>0.5625</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="4">
         <v>0.4883720874786377</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="4">
         <v>0.20000000298023221</v>
       </c>
       <c r="V7">
@@ -3127,7 +3095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3137,58 +3105,58 @@
       <c r="C8">
         <v>22</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>0.86179880915073648</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>0.85910105196047182</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>0.87118643522262573</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>0.92343389987945557</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <v>0.90754258632659912</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <v>0.74712646007537842</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="5">
         <v>0.78200691938400269</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>0.60000002384185791</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <v>0.75</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="5">
         <v>0.4375</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="4">
         <v>0.88827329874038696</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="4">
         <v>0.93049329519271851</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="5">
         <v>0.89847713708877563</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="5">
         <v>0.71465969085693359</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="4">
         <v>0.82156133651733398</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="5">
         <v>0.5</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V8">
@@ -3198,7 +3166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3208,58 +3176,58 @@
       <c r="C9">
         <v>25</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>0.8480100282043247</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>0.84093082562958243</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>0.87203389406204224</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="4">
         <v>0.92111366987228394</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>0.88077861070632935</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <v>0.62931036949157715</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="5">
         <v>0.81660902500152588</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="5">
         <v>0.47999998927116388</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="5">
         <v>0.76666665077209473</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="5">
         <v>0.5</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="4">
         <v>0.88919669389724731</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="4">
         <v>0.92264574766159058</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="5">
         <v>0.84771573543548584</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="5">
         <v>0.62827223539352417</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="4">
         <v>0.82527881860733032</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="5">
         <v>0.625</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="5">
         <v>0.5116279125213623</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="5">
         <v>0.13333334028720861</v>
       </c>
       <c r="V9">
@@ -3279,58 +3247,58 @@
       <c r="C10">
         <v>42</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>0.8241930429332498</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>0.81734140898948038</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>0.83389830589294434</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="4">
         <v>0.90719258785247803</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>0.87347930669784546</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <v>0.68678158521652222</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="5">
         <v>0.74740487337112427</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>0.40000000596046448</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <v>0.56666666269302368</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <v>0.375</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="4">
         <v>0.81902122497558594</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="4">
         <v>0.91143494844436646</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="5">
         <v>0.85532993078231812</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="5">
         <v>0.67801046371459961</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="4">
         <v>0.81040894985198975</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="5">
         <v>0.5</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="5">
         <v>0.45348837971687322</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V10">
@@ -3340,7 +3308,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3350,58 +3318,58 @@
       <c r="C11">
         <v>31</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>0.81353807583829518</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>0.80745935607268093</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>0.81779658794403076</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <v>0.89327144622802734</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>0.81995135545730591</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>0.68103450536727905</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="5">
         <v>0.77854669094085693</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>0.43999999761581421</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="5">
         <v>0.75</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="5">
         <v>0.375</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="4">
         <v>0.811634361743927</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="4">
         <v>0.89686095714569092</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="5">
         <v>0.80456852912902832</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="5">
         <v>0.67015707492828369</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="4">
         <v>0.80297398567199707</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="5">
         <v>0.5</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="5">
         <v>0.62790697813034058</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V11">
@@ -3411,7 +3379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3421,58 +3389,58 @@
       <c r="C12">
         <v>27</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>0.82544656847383269</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>0.82116671979598344</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>0.83050847053527832</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="4">
         <v>0.90719258785247803</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>0.87834548950195313</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <v>0.69540232419967651</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="5">
         <v>0.754325270652771</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>0.43999999761581421</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="5">
         <v>0.56666666269302368</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="5">
         <v>0.375</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="4">
         <v>0.84025853872299194</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="4">
         <v>0.89798206090927124</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="5">
         <v>0.84517765045166016</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="5">
         <v>0.69109946489334106</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="4">
         <v>0.78810411691665649</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="5">
         <v>0.5116279125213623</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V12">
@@ -3482,7 +3450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3492,58 +3460,58 @@
       <c r="C13">
         <v>41</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>0.78470698840488873</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>0.77398788651577943</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>0.75423729419708252</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="4">
         <v>0.88747102022171021</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>0.87834548950195313</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <v>0.64367818832397461</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="5">
         <v>0.73702424764633179</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="5">
         <v>0.43999999761581421</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="5">
         <v>0.56666666269302368</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="5">
         <v>0.375</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="4">
         <v>0.75623267889022827</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="4">
         <v>0.87556052207946777</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="5">
         <v>0.85532993078231812</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="5">
         <v>0.60209423303604126</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="4">
         <v>0.78810411691665649</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="5">
         <v>0.43023255467414862</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V13">
@@ -3563,58 +3531,58 @@
       <c r="C14">
         <v>26</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>0.82795361955499847</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>0.81734140898948038</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <v>0.82288134098052979</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="4">
         <v>0.91067284345626831</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>0.88077861070632935</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>0.71264368295669556</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="5">
         <v>0.78200691938400269</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>0.40000000596046448</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="5">
         <v>0.56666666269302368</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="5">
         <v>0.375</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="4">
         <v>0.81440442800521851</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="4">
         <v>0.9035874605178833</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="5">
         <v>0.88324874639511108</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="5">
         <v>0.67277485132217407</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="4">
         <v>0.81040894985198975</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="5">
         <v>0.5</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="5">
         <v>0.4883720874786377</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V14">
@@ -3624,7 +3592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3634,58 +3602,58 @@
       <c r="C15">
         <v>23</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>0.8110310247571294</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>0.80682180427159711</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="5">
         <v>0.81525421142578125</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="4">
         <v>0.89095127582550049</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>0.79318732023239136</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <v>0.71551722288131714</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="5">
         <v>0.75778543949127197</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="5">
         <v>0.63999998569488525</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="5">
         <v>0.68333333730697632</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="5">
         <v>0.4375</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="4">
         <v>0.81255769729614258</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="4">
         <v>0.89910316467285156</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="5">
         <v>0.78680205345153809</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="5">
         <v>0.68324607610702515</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="4">
         <v>0.79925650358200073</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="5">
         <v>0.625</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="5">
         <v>0.56976741552352905</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="5">
         <v>0.26666668057441711</v>
       </c>
       <c r="V15">
@@ -3695,7 +3663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3705,58 +3673,58 @@
       <c r="C16">
         <v>56</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>0.84550297712315892</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>0.84475613643608538</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5">
         <v>0.85593217611312866</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>0.93271464109420776</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>0.89537709951400757</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="5">
         <v>0.70114940404891968</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="5">
         <v>0.74740487337112427</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="5">
         <v>0.40000000596046448</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="5">
         <v>0.64999997615814209</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="5">
         <v>0.4375</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="4">
         <v>0.87442290782928467</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="4">
         <v>0.93834078311920166</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="5">
         <v>0.88578683137893677</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="5">
         <v>0.65968585014343262</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="4">
         <v>0.78810411691665649</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="5">
         <v>0.5</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="5">
         <v>0.4883720874786377</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V16">
@@ -3766,7 +3734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3776,58 +3744,58 @@
       <c r="C17">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <v>0.56283296772171731</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>0.52502390819254063</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="5">
         <v>0.61779659986495972</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="4">
         <v>0.56496518850326538</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>0.66909974813461304</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="5">
         <v>0.33908045291900629</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="5">
         <v>0.45328718423843378</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="5">
         <v>0.47999998927116388</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="5">
         <v>0.58333331346511841</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="4">
         <v>0.59556788206100464</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="4">
         <v>0.53363227844238281</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="5">
         <v>0.63197970390319824</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="5">
         <v>0.28795811533927917</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R17" s="4">
         <v>0.43122676014900208</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="5">
         <v>0.45348837971687322</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V17">
@@ -3847,58 +3815,58 @@
       <c r="C18">
         <v>42</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>0.75180194296458791</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>0.7494421421740517</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="5">
         <v>0.67627120018005371</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="4">
         <v>0.84918791055679321</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>0.86861312389373779</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <v>0.70977014303207397</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="5">
         <v>0.72318339347839355</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="5">
         <v>0.43999999761581421</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="5">
         <v>0.64999997615814209</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="5">
         <v>0.375</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="4">
         <v>0.6694367527961731</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="4">
         <v>0.85201793909072876</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="5">
         <v>0.86802029609680176</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="5">
         <v>0.68848168849945068</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R18" s="4">
         <v>0.77695167064666748</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="5">
         <v>0.5</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="5">
         <v>0.47674417495727539</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V18">
@@ -3908,7 +3876,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -3918,58 +3886,58 @@
       <c r="C19">
         <v>42</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <v>0.75368223127546219</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>0.7484858144724259</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="5">
         <v>0.7127118706703186</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="4">
         <v>0.86542922258377075</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>0.84914839267730713</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <v>0.59770113229751587</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="5">
         <v>0.69550174474716187</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="5">
         <v>0.51999998092651367</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="5">
         <v>0.64999997615814209</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="5">
         <v>0.5</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="4">
         <v>0.72022157907485962</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="4">
         <v>0.85313904285430908</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="5">
         <v>0.8350253701210022</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="5">
         <v>0.57329845428466797</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R19" s="4">
         <v>0.75836431980133057</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="5">
         <v>0.6875</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="5">
         <v>0.47674417495727539</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V19">
@@ -3979,7 +3947,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -3989,58 +3957,58 @@
       <c r="C20">
         <v>55</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <v>0.75744280789721086</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>0.74784826267134208</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5">
         <v>0.72372883558273315</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="4">
         <v>0.86542922258377075</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>0.82968372106552124</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="5">
         <v>0.60344827175140381</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="5">
         <v>0.70242214202880859</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="5">
         <v>0.60000002384185791</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="5">
         <v>0.63333332538604736</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="5">
         <v>0.625</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="4">
         <v>0.72945523262023926</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="4">
         <v>0.8464125394821167</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="5">
         <v>0.7842639684677124</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="5">
         <v>0.6073298454284668</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20" s="4">
         <v>0.73605948686599731</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="5">
         <v>0.625</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="5">
         <v>0.58139532804489136</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="5">
         <v>0.13333334028720861</v>
       </c>
       <c r="V20">
@@ -4050,7 +4018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -4060,58 +4028,58 @@
       <c r="C21">
         <v>40</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="5">
         <v>0.76308367282983391</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>0.76697481670385714</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="5">
         <v>0.73220336437225342</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="4">
         <v>0.82946634292602539</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <v>0.86131387948989868</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="5">
         <v>0.66954022645950317</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="5">
         <v>0.73356401920318604</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="5">
         <v>0.47999998927116388</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="5">
         <v>0.64999997615814209</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="5">
         <v>0.375</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="4">
         <v>0.73868882656097412</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O21" s="4">
         <v>0.86547082662582397</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="5">
         <v>0.81979697942733765</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="5">
         <v>0.65968585014343262</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R21" s="4">
         <v>0.75836431980133057</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="5">
         <v>0.5116279125213623</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="5">
         <v>0.13333334028720861</v>
       </c>
       <c r="V21">
@@ -4131,58 +4099,58 @@
       <c r="C22">
         <v>36</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="5">
         <v>0.77060482607333125</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>0.76665604080331529</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="5">
         <v>0.75593221187591553</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="4">
         <v>0.87238979339599609</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <v>0.79805350303649902</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="5">
         <v>0.68678158521652222</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="5">
         <v>0.6747404932975769</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="5">
         <v>0.43999999761581421</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="5">
         <v>0.60000002384185791</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="5">
         <v>0.375</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="4">
         <v>0.76638966798782349</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O22" s="4">
         <v>0.85089683532714844</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="5">
         <v>0.7842639684677124</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="5">
         <v>0.67015707492828369</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R22" s="4">
         <v>0.72118961811065674</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="5">
         <v>0.625</v>
       </c>
-      <c r="T22">
+      <c r="T22" s="5">
         <v>0.5116279125213623</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V22">
@@ -4192,7 +4160,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -4202,58 +4170,58 @@
       <c r="C23">
         <v>42</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="5">
         <v>0.79191476026324037</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>0.78163850812878544</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <v>0.76355934143066406</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="4">
         <v>0.88283061981201172</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>0.85158151388168335</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="5">
         <v>0.69252872467041016</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="5">
         <v>0.75778543949127197</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="5">
         <v>0.47999998927116388</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="5">
         <v>0.56666666269302368</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="5">
         <v>0.5625</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="4">
         <v>0.76269620656967163</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23" s="4">
         <v>0.87107622623443604</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="5">
         <v>0.82741117477416992</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="5">
         <v>0.66492146253585815</v>
       </c>
-      <c r="R23" s="2">
+      <c r="R23" s="4">
         <v>0.78810411691665649</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="5">
         <v>0.6875</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="5">
         <v>0.5</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V23">
@@ -4263,7 +4231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -4273,58 +4241,58 @@
       <c r="C24">
         <v>50</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="5">
         <v>0.81353807583829518</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>0.80586547656997132</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="5">
         <v>0.79237288236618042</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="4">
         <v>0.90719258785247803</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="5">
         <v>0.85888075828552246</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="5">
         <v>0.69252872467041016</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="5">
         <v>0.76124566793441772</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="5">
         <v>0.47999998927116388</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="5">
         <v>0.71666663885116577</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="5">
         <v>0.625</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="4">
         <v>0.80240076780319214</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="4">
         <v>0.90246635675430298</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="5">
         <v>0.8350253701210022</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="5">
         <v>0.67277485132217407</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R24" s="4">
         <v>0.76579928398132324</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="5">
         <v>0.56976741552352905</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="5">
         <v>0.26666668057441711</v>
       </c>
       <c r="V24">
@@ -4334,7 +4302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -4344,58 +4312,58 @@
       <c r="C25">
         <v>42</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="5">
         <v>0.79880915073644621</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>0.79247688874721067</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="5">
         <v>0.78644067049026489</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="4">
         <v>0.88515079021453857</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>0.88077861070632935</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="5">
         <v>0.66666668653488159</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="5">
         <v>0.73356401920318604</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="5">
         <v>0.43999999761581421</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="5">
         <v>0.53333336114883423</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="5">
         <v>0.5625</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="4">
         <v>0.78670358657836914</v>
       </c>
-      <c r="O25" s="2">
+      <c r="O25" s="4">
         <v>0.88452917337417603</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="5">
         <v>0.84771573543548584</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="5">
         <v>0.65445023775100708</v>
       </c>
-      <c r="R25" s="2">
+      <c r="R25" s="4">
         <v>0.77695167064666748</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="5">
         <v>0.5625</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="5">
         <v>0.46511629223823547</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="5">
         <v>0.20000000298023221</v>
       </c>
       <c r="V25">
@@ -4405,37 +4373,183 @@
         <v>33</v>
       </c>
     </row>
-    <row r="1048559" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D1048559" s="1"/>
-      <c r="E1048559" s="1"/>
-      <c r="F1048559" s="1"/>
-      <c r="H1048559" s="1"/>
-      <c r="I1048559" s="1"/>
-      <c r="J1048559" s="1"/>
-      <c r="K1048559" s="1"/>
-      <c r="L1048559" s="1"/>
-      <c r="M1048559" s="1"/>
-      <c r="P1048559" s="1"/>
-      <c r="Q1048559" s="1"/>
-      <c r="S1048559" s="1"/>
-      <c r="T1048559" s="1"/>
-      <c r="U1048559" s="1"/>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.90668202764976957</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.90998268897864976</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.82788527011871338</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0.88318228721618652</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.78842675685882568</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0.47179487347602839</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.63636362552642822</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0.32867133617401117</v>
+      </c>
+      <c r="M27" s="4">
+        <v>7.2727270424365997E-2</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0.83080112934112549</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0.89009898900985718</v>
+      </c>
+      <c r="P27" s="4">
+        <v>0.75963300466537476</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>0.44476744532585138</v>
+      </c>
+      <c r="R27" s="4">
+        <v>0.68733853101730347</v>
+      </c>
+      <c r="S27" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="T27" s="4">
+        <v>0.29213482141494751</v>
+      </c>
+      <c r="U27" s="4">
+        <v>0.1025641039013863</v>
+      </c>
+      <c r="V27">
+        <v>64</v>
+      </c>
+      <c r="W27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0.907258064516129</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.90767455279861509</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.80920612812042236</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.86002016067504883</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.79746836423873901</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0.60000002384185791</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0.61616164445877075</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0.26666668057441711</v>
+      </c>
+      <c r="L28" s="5">
+        <v>0.20979021489620209</v>
+      </c>
+      <c r="M28" s="5">
+        <v>1.8181817606091499E-2</v>
+      </c>
+      <c r="N28" s="5">
+        <v>0.81491714715957642</v>
+      </c>
+      <c r="O28" s="5">
+        <v>0.86336636543273926</v>
+      </c>
+      <c r="P28" s="5">
+        <v>0.80000001192092896</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>0.53488373756408691</v>
+      </c>
+      <c r="R28" s="5">
+        <v>0.63824290037155151</v>
+      </c>
+      <c r="S28" s="5">
+        <v>0.17499999701976779</v>
+      </c>
+      <c r="T28" s="5">
+        <v>0.19662921130657199</v>
+      </c>
+      <c r="U28" s="5">
+        <v>2.5641025975346569E-2</v>
+      </c>
+      <c r="V28">
+        <v>64</v>
+      </c>
+      <c r="W28" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="1048560" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D1048560" s="2"/>
-      <c r="E1048560" s="2"/>
-      <c r="F1048560" s="2"/>
-      <c r="H1048560" s="2"/>
-      <c r="I1048560" s="2"/>
-      <c r="J1048560" s="2"/>
-      <c r="K1048560" s="2"/>
-      <c r="L1048560" s="2"/>
-      <c r="M1048560" s="2"/>
-      <c r="P1048560" s="2"/>
-      <c r="Q1048560" s="2"/>
-      <c r="S1048560" s="2"/>
-      <c r="T1048560" s="2"/>
-      <c r="U1048560" s="2"/>
+      <c r="D1048560" s="1"/>
+      <c r="E1048560" s="1"/>
+      <c r="F1048560" s="1"/>
+      <c r="H1048560" s="1"/>
+      <c r="I1048560" s="1"/>
+      <c r="J1048560" s="1"/>
+      <c r="K1048560" s="1"/>
+      <c r="L1048560" s="1"/>
+      <c r="M1048560" s="1"/>
+      <c r="P1048560" s="1"/>
+      <c r="Q1048560" s="1"/>
+      <c r="S1048560" s="1"/>
+      <c r="T1048560" s="1"/>
+      <c r="U1048560" s="1"/>
     </row>
     <row r="1048561" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D1048561" s="2"/>
@@ -4517,66 +4631,76 @@
       <c r="T1048565" s="2"/>
       <c r="U1048565" s="2"/>
     </row>
+    <row r="1048566" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D1048566" s="2"/>
+      <c r="E1048566" s="2"/>
+      <c r="F1048566" s="2"/>
+      <c r="H1048566" s="2"/>
+      <c r="I1048566" s="2"/>
+      <c r="J1048566" s="2"/>
+      <c r="K1048566" s="2"/>
+      <c r="L1048566" s="2"/>
+      <c r="M1048566" s="2"/>
+      <c r="P1048566" s="2"/>
+      <c r="Q1048566" s="2"/>
+      <c r="S1048566" s="2"/>
+      <c r="T1048566" s="2"/>
+      <c r="U1048566" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:B94" xr:uid="{00000000-0001-0000-2400-000000000000}">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="majority"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <conditionalFormatting sqref="G2:G25">
-    <cfRule type="top10" dxfId="30" priority="31" rank="1"/>
+  <autoFilter ref="B1:B95" xr:uid="{00000000-0001-0000-2400-000000000000}"/>
+  <conditionalFormatting sqref="D1048561:D1048566 D2:D7">
+    <cfRule type="top10" dxfId="17" priority="16" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N25">
-    <cfRule type="top10" dxfId="23" priority="24" rank="1"/>
+  <conditionalFormatting sqref="E1048561:E1048566 E2:E7">
+    <cfRule type="top10" dxfId="16" priority="15" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O25">
-    <cfRule type="top10" dxfId="22" priority="23" rank="1"/>
+  <conditionalFormatting sqref="F1048561:F1048566 F2:F7">
+    <cfRule type="top10" dxfId="15" priority="13" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R25">
-    <cfRule type="top10" dxfId="20" priority="21" rank="1"/>
+  <conditionalFormatting sqref="G2:G26">
+    <cfRule type="top10" dxfId="14" priority="31" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1048560:D1048565 D2:D7">
-    <cfRule type="top10" dxfId="15" priority="16" rank="1"/>
+  <conditionalFormatting sqref="H1048561:H1048566 H2:H7">
+    <cfRule type="top10" dxfId="13" priority="12" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1048560:E1048565 E2:E7">
-    <cfRule type="top10" dxfId="14" priority="15" rank="1"/>
+  <conditionalFormatting sqref="I1048561:I1048566 I2:I7">
+    <cfRule type="top10" dxfId="12" priority="10" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1048560:F1048565 F2:F7">
-    <cfRule type="top10" dxfId="12" priority="13" rank="1"/>
+  <conditionalFormatting sqref="J1048561:J1048566 J2:J7">
+    <cfRule type="top10" dxfId="11" priority="9" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1048560:H1048565 H2:H7">
-    <cfRule type="top10" dxfId="11" priority="12" rank="1"/>
+  <conditionalFormatting sqref="K1048561:K1048566 K2:K7">
+    <cfRule type="top10" dxfId="10" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1048560:I1048565 I2:I7">
-    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
+  <conditionalFormatting sqref="L1048561:L1048566 L2:L7">
+    <cfRule type="top10" dxfId="9" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1048560:J1048565 J2:J7">
-    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
+  <conditionalFormatting sqref="M1048561:M1048566 M2:M7">
+    <cfRule type="top10" dxfId="8" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1048560:K1048565 K2:K7">
-    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+  <conditionalFormatting sqref="N2:N26">
+    <cfRule type="top10" dxfId="7" priority="24" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1048560:L1048565 L2:L7">
-    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+  <conditionalFormatting sqref="O2:O26">
+    <cfRule type="top10" dxfId="6" priority="23" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1048560:M1048565 M2:M7">
-    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
+  <conditionalFormatting sqref="P1048561:P1048566 P2:P7">
+    <cfRule type="top10" dxfId="5" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1048560:P1048565 P2:P7">
-    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+  <conditionalFormatting sqref="Q1048561:Q1048566 Q2:Q7">
+    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1048560:Q1048565 Q2:Q7">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+  <conditionalFormatting sqref="R2:R26">
+    <cfRule type="top10" dxfId="3" priority="21" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1048560:S1048565 S2:S7">
+  <conditionalFormatting sqref="S1048561:S1048566 S2:S7">
     <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1048560:T1048565 T2:T7">
+  <conditionalFormatting sqref="T1048561:T1048566 T2:T7">
     <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1048560:U1048565 U2:U7">
+  <conditionalFormatting sqref="U1048561:U1048566 U2:U7">
     <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>